<commit_message>
lay ten dang nhap
</commit_message>
<xml_diff>
--- a/ExcelXuatVaoDay/nv.xlsx
+++ b/ExcelXuatVaoDay/nv.xlsx
@@ -1069,16 +1069,9 @@
       <x:c r="J21" s="9"/>
     </x:row>
     <x:row r="22" spans="1:10">
-      <x:c r="H22" s="9" t="s">
+      <x:c r="H22" s="0" t="s">
         <x:v>67</x:v>
       </x:c>
-      <x:c r="I22" s="9"/>
-      <x:c r="J22" s="9"/>
-    </x:row>
-    <x:row r="23" spans="1:10">
-      <x:c r="H23" s="9"/>
-      <x:c r="I23" s="9"/>
-      <x:c r="J23" s="9"/>
     </x:row>
     <x:row r="24" spans="1:10">
       <x:c r="H24" s="9"/>
@@ -1092,7 +1085,7 @@
     <x:mergeCell ref="A8:J8"/>
     <x:mergeCell ref="H20:J20"/>
     <x:mergeCell ref="H21:J21"/>
-    <x:mergeCell ref="H22:J24"/>
+    <x:mergeCell ref="H24:J24"/>
   </x:mergeCells>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>